<commit_message>
added some unit tests
</commit_message>
<xml_diff>
--- a/data/leaf_CNP/Soil and Leaf Analysis SVS October 2016.xlsx
+++ b/data/leaf_CNP/Soil and Leaf Analysis SVS October 2016.xlsx
@@ -2774,8 +2774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2833,7 +2833,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>724</v>
+        <v>717</v>
       </c>
       <c r="C3">
         <v>355.88799999999998</v>
@@ -3593,7 +3593,7 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>717</v>
+        <v>724</v>
       </c>
       <c r="C41">
         <v>120.611</v>

</xml_diff>